<commit_message>
Atualizado por script em 21-11-2023 14:30
</commit_message>
<xml_diff>
--- a/2023/poland_iii-liga-group-iv_2023-2024.xlsx
+++ b/2023/poland_iii-liga-group-iv_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V133"/>
+  <dimension ref="A1:V134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6461,22 +6461,22 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Orleta Radzyn</t>
+          <t>Chelmianka Chelm</t>
         </is>
       </c>
       <c r="G66" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Podhale Nowy Targ</t>
+          <t>Star Starachowice</t>
         </is>
       </c>
       <c r="I66" t="n">
         <v>0</v>
       </c>
       <c r="J66" t="n">
-        <v>3.04</v>
+        <v>2.1</v>
       </c>
       <c r="K66" t="inlineStr">
         <is>
@@ -6484,15 +6484,15 @@
         </is>
       </c>
       <c r="L66" t="n">
-        <v>2.77</v>
+        <v>2.6</v>
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>23/09/2023 15:13</t>
+          <t>23/09/2023 15:08</t>
         </is>
       </c>
       <c r="N66" t="n">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -6500,15 +6500,15 @@
         </is>
       </c>
       <c r="P66" t="n">
-        <v>3.6</v>
+        <v>3.37</v>
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>23/09/2023 15:13</t>
+          <t>23/09/2023 15:08</t>
         </is>
       </c>
       <c r="R66" t="n">
-        <v>1.9</v>
+        <v>2.8</v>
       </c>
       <c r="S66" t="inlineStr">
         <is>
@@ -6516,16 +6516,16 @@
         </is>
       </c>
       <c r="T66" t="n">
-        <v>2.14</v>
+        <v>2.36</v>
       </c>
       <c r="U66" t="inlineStr">
         <is>
-          <t>23/09/2023 15:13</t>
+          <t>23/09/2023 15:08</t>
         </is>
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/orleta-radzyn-podhale-nowy-targ/CSen0uO1/</t>
+          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/chelmianka-chelm-star-starachowice/KUG77NVR/</t>
         </is>
       </c>
     </row>
@@ -6553,22 +6553,22 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Chelmianka Chelm</t>
+          <t>Orleta Radzyn</t>
         </is>
       </c>
       <c r="G67" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Star Starachowice</t>
+          <t>Podhale Nowy Targ</t>
         </is>
       </c>
       <c r="I67" t="n">
         <v>0</v>
       </c>
       <c r="J67" t="n">
-        <v>2.1</v>
+        <v>3.04</v>
       </c>
       <c r="K67" t="inlineStr">
         <is>
@@ -6576,15 +6576,15 @@
         </is>
       </c>
       <c r="L67" t="n">
-        <v>2.6</v>
+        <v>2.77</v>
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>23/09/2023 15:08</t>
+          <t>23/09/2023 15:13</t>
         </is>
       </c>
       <c r="N67" t="n">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -6592,15 +6592,15 @@
         </is>
       </c>
       <c r="P67" t="n">
-        <v>3.37</v>
+        <v>3.6</v>
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>23/09/2023 15:08</t>
+          <t>23/09/2023 15:13</t>
         </is>
       </c>
       <c r="R67" t="n">
-        <v>2.8</v>
+        <v>1.9</v>
       </c>
       <c r="S67" t="inlineStr">
         <is>
@@ -6608,16 +6608,16 @@
         </is>
       </c>
       <c r="T67" t="n">
-        <v>2.36</v>
+        <v>2.14</v>
       </c>
       <c r="U67" t="inlineStr">
         <is>
-          <t>23/09/2023 15:08</t>
+          <t>23/09/2023 15:13</t>
         </is>
       </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/chelmianka-chelm-star-starachowice/KUG77NVR/</t>
+          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/orleta-radzyn-podhale-nowy-targ/CSen0uO1/</t>
         </is>
       </c>
     </row>
@@ -7657,22 +7657,22 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Avia Swidnik</t>
+          <t>Unia Tarnow</t>
         </is>
       </c>
       <c r="G79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Karpaty Krosno</t>
+          <t>Podhale Nowy Targ</t>
         </is>
       </c>
       <c r="I79" t="n">
         <v>1</v>
       </c>
       <c r="J79" t="n">
-        <v>1.2</v>
+        <v>2.56</v>
       </c>
       <c r="K79" t="inlineStr">
         <is>
@@ -7680,15 +7680,15 @@
         </is>
       </c>
       <c r="L79" t="n">
-        <v>1.15</v>
+        <v>2.77</v>
       </c>
       <c r="M79" t="inlineStr">
         <is>
-          <t>07/10/2023 13:04</t>
+          <t>07/10/2023 14:59</t>
         </is>
       </c>
       <c r="N79" t="n">
-        <v>5.31</v>
+        <v>3.21</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
@@ -7696,15 +7696,15 @@
         </is>
       </c>
       <c r="P79" t="n">
-        <v>6.81</v>
+        <v>3.77</v>
       </c>
       <c r="Q79" t="inlineStr">
         <is>
-          <t>07/10/2023 14:12</t>
+          <t>07/10/2023 14:59</t>
         </is>
       </c>
       <c r="R79" t="n">
-        <v>7.58</v>
+        <v>2.25</v>
       </c>
       <c r="S79" t="inlineStr">
         <is>
@@ -7712,16 +7712,16 @@
         </is>
       </c>
       <c r="T79" t="n">
-        <v>10.98</v>
+        <v>2.09</v>
       </c>
       <c r="U79" t="inlineStr">
         <is>
-          <t>07/10/2023 14:12</t>
+          <t>07/10/2023 14:59</t>
         </is>
       </c>
       <c r="V79" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/avia-swidnik-ks-karpaty-krosno/K6rv2MAn/</t>
+          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/unia-tarnow-podhale-nowy-targ/SxZbcbPH/</t>
         </is>
       </c>
     </row>
@@ -7749,22 +7749,22 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Garbarnia</t>
+          <t>Avia Swidnik</t>
         </is>
       </c>
       <c r="G80" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Sokol Sieniawa</t>
+          <t>Karpaty Krosno</t>
         </is>
       </c>
       <c r="I80" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J80" t="n">
-        <v>1.28</v>
+        <v>1.2</v>
       </c>
       <c r="K80" t="inlineStr">
         <is>
@@ -7772,15 +7772,15 @@
         </is>
       </c>
       <c r="L80" t="n">
-        <v>1.29</v>
+        <v>1.15</v>
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>07/10/2023 14:57</t>
+          <t>07/10/2023 13:04</t>
         </is>
       </c>
       <c r="N80" t="n">
-        <v>4.9</v>
+        <v>5.31</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
@@ -7788,15 +7788,15 @@
         </is>
       </c>
       <c r="P80" t="n">
-        <v>5.5</v>
+        <v>6.81</v>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
-          <t>07/10/2023 14:57</t>
+          <t>07/10/2023 14:12</t>
         </is>
       </c>
       <c r="R80" t="n">
-        <v>6.08</v>
+        <v>7.58</v>
       </c>
       <c r="S80" t="inlineStr">
         <is>
@@ -7804,16 +7804,16 @@
         </is>
       </c>
       <c r="T80" t="n">
-        <v>6.65</v>
+        <v>10.98</v>
       </c>
       <c r="U80" t="inlineStr">
         <is>
-          <t>07/10/2023 14:57</t>
+          <t>07/10/2023 14:12</t>
         </is>
       </c>
       <c r="V80" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/garbarnia-sokol-sieniawa/0M177rmP/</t>
+          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/avia-swidnik-ks-karpaty-krosno/K6rv2MAn/</t>
         </is>
       </c>
     </row>
@@ -7841,22 +7841,22 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Orleta Radzyn</t>
+          <t>Garbarnia</t>
         </is>
       </c>
       <c r="G81" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Siarka Tarnobrzeg</t>
+          <t>Sokol Sieniawa</t>
         </is>
       </c>
       <c r="I81" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J81" t="n">
-        <v>5.53</v>
+        <v>1.28</v>
       </c>
       <c r="K81" t="inlineStr">
         <is>
@@ -7864,15 +7864,15 @@
         </is>
       </c>
       <c r="L81" t="n">
-        <v>4.81</v>
+        <v>1.29</v>
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>07/10/2023 14:07</t>
+          <t>07/10/2023 14:57</t>
         </is>
       </c>
       <c r="N81" t="n">
-        <v>4.48</v>
+        <v>4.9</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
@@ -7880,15 +7880,15 @@
         </is>
       </c>
       <c r="P81" t="n">
-        <v>3.67</v>
+        <v>5.5</v>
       </c>
       <c r="Q81" t="inlineStr">
         <is>
-          <t>07/10/2023 14:07</t>
+          <t>07/10/2023 14:57</t>
         </is>
       </c>
       <c r="R81" t="n">
-        <v>1.34</v>
+        <v>6.08</v>
       </c>
       <c r="S81" t="inlineStr">
         <is>
@@ -7896,16 +7896,16 @@
         </is>
       </c>
       <c r="T81" t="n">
-        <v>1.6</v>
+        <v>6.65</v>
       </c>
       <c r="U81" t="inlineStr">
         <is>
-          <t>07/10/2023 14:07</t>
+          <t>07/10/2023 14:57</t>
         </is>
       </c>
       <c r="V81" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/orleta-radzyn-siarka-tarnobrzeg/6NpjaKf5/</t>
+          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/garbarnia-sokol-sieniawa/0M177rmP/</t>
         </is>
       </c>
     </row>
@@ -7933,22 +7933,22 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Unia Tarnow</t>
+          <t>Orleta Radzyn</t>
         </is>
       </c>
       <c r="G82" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Podhale Nowy Targ</t>
+          <t>Siarka Tarnobrzeg</t>
         </is>
       </c>
       <c r="I82" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J82" t="n">
-        <v>2.56</v>
+        <v>5.53</v>
       </c>
       <c r="K82" t="inlineStr">
         <is>
@@ -7956,15 +7956,15 @@
         </is>
       </c>
       <c r="L82" t="n">
-        <v>2.77</v>
+        <v>4.81</v>
       </c>
       <c r="M82" t="inlineStr">
         <is>
-          <t>07/10/2023 14:59</t>
+          <t>07/10/2023 14:07</t>
         </is>
       </c>
       <c r="N82" t="n">
-        <v>3.21</v>
+        <v>4.48</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -7972,15 +7972,15 @@
         </is>
       </c>
       <c r="P82" t="n">
-        <v>3.77</v>
+        <v>3.67</v>
       </c>
       <c r="Q82" t="inlineStr">
         <is>
-          <t>07/10/2023 14:59</t>
+          <t>07/10/2023 14:07</t>
         </is>
       </c>
       <c r="R82" t="n">
-        <v>2.25</v>
+        <v>1.34</v>
       </c>
       <c r="S82" t="inlineStr">
         <is>
@@ -7988,16 +7988,16 @@
         </is>
       </c>
       <c r="T82" t="n">
-        <v>2.09</v>
+        <v>1.6</v>
       </c>
       <c r="U82" t="inlineStr">
         <is>
-          <t>07/10/2023 14:59</t>
+          <t>07/10/2023 14:07</t>
         </is>
       </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/unia-tarnow-podhale-nowy-targ/SxZbcbPH/</t>
+          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/orleta-radzyn-siarka-tarnobrzeg/6NpjaKf5/</t>
         </is>
       </c>
     </row>
@@ -8577,71 +8577,71 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Siarka Tarnobrzeg</t>
+          <t>Swidniczanka Swidnik</t>
         </is>
       </c>
       <c r="G89" t="n">
+        <v>3</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Unia Tarnow</t>
+        </is>
+      </c>
+      <c r="I89" t="n">
         <v>2</v>
       </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>Ostrowiec Swietokrzyski</t>
-        </is>
-      </c>
-      <c r="I89" t="n">
-        <v>0</v>
-      </c>
       <c r="J89" t="n">
-        <v>1.57</v>
+        <v>1.95</v>
       </c>
       <c r="K89" t="inlineStr">
         <is>
-          <t>13/10/2023 02:13</t>
+          <t>14/10/2023 09:43</t>
         </is>
       </c>
       <c r="L89" t="n">
-        <v>1.61</v>
+        <v>1.91</v>
       </c>
       <c r="M89" t="inlineStr">
         <is>
-          <t>14/10/2023 14:07</t>
+          <t>14/10/2023 14:47</t>
         </is>
       </c>
       <c r="N89" t="n">
-        <v>3.65</v>
+        <v>3.5</v>
       </c>
       <c r="O89" t="inlineStr">
         <is>
-          <t>13/10/2023 02:13</t>
+          <t>14/10/2023 09:43</t>
         </is>
       </c>
       <c r="P89" t="n">
-        <v>3.53</v>
+        <v>3.58</v>
       </c>
       <c r="Q89" t="inlineStr">
         <is>
-          <t>14/10/2023 14:08</t>
+          <t>14/10/2023 14:47</t>
         </is>
       </c>
       <c r="R89" t="n">
-        <v>4.17</v>
+        <v>3.18</v>
       </c>
       <c r="S89" t="inlineStr">
         <is>
-          <t>13/10/2023 02:13</t>
+          <t>14/10/2023 09:43</t>
         </is>
       </c>
       <c r="T89" t="n">
-        <v>4.99</v>
+        <v>3.31</v>
       </c>
       <c r="U89" t="inlineStr">
         <is>
-          <t>14/10/2023 14:07</t>
+          <t>14/10/2023 14:47</t>
         </is>
       </c>
       <c r="V89" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/siarka-tarnobrzeg-ostrowiec-swietokrzyski/ns2LEafh/</t>
+          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/swidniczanka-swidnik-unia-tarnow/hK2HFuun/</t>
         </is>
       </c>
     </row>
@@ -8669,22 +8669,22 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Star Starachowice</t>
+          <t>Siarka Tarnobrzeg</t>
         </is>
       </c>
       <c r="G90" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Biala Podlaska</t>
+          <t>Ostrowiec Swietokrzyski</t>
         </is>
       </c>
       <c r="I90" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J90" t="n">
-        <v>2.06</v>
+        <v>1.57</v>
       </c>
       <c r="K90" t="inlineStr">
         <is>
@@ -8692,15 +8692,15 @@
         </is>
       </c>
       <c r="L90" t="n">
-        <v>1.95</v>
+        <v>1.61</v>
       </c>
       <c r="M90" t="inlineStr">
         <is>
-          <t>14/10/2023 00:21</t>
+          <t>14/10/2023 14:07</t>
         </is>
       </c>
       <c r="N90" t="n">
-        <v>3.25</v>
+        <v>3.65</v>
       </c>
       <c r="O90" t="inlineStr">
         <is>
@@ -8708,15 +8708,15 @@
         </is>
       </c>
       <c r="P90" t="n">
-        <v>3.26</v>
+        <v>3.53</v>
       </c>
       <c r="Q90" t="inlineStr">
         <is>
-          <t>14/10/2023 13:02</t>
+          <t>14/10/2023 14:08</t>
         </is>
       </c>
       <c r="R90" t="n">
-        <v>2.83</v>
+        <v>4.17</v>
       </c>
       <c r="S90" t="inlineStr">
         <is>
@@ -8724,16 +8724,16 @@
         </is>
       </c>
       <c r="T90" t="n">
-        <v>3.44</v>
+        <v>4.99</v>
       </c>
       <c r="U90" t="inlineStr">
         <is>
-          <t>14/10/2023 00:21</t>
+          <t>14/10/2023 14:07</t>
         </is>
       </c>
       <c r="V90" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/star-starachowice-biala-podlaska/r9eUCwP4/</t>
+          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/siarka-tarnobrzeg-ostrowiec-swietokrzyski/ns2LEafh/</t>
         </is>
       </c>
     </row>
@@ -8761,71 +8761,71 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Swidniczanka Swidnik</t>
+          <t>Star Starachowice</t>
         </is>
       </c>
       <c r="G91" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>Unia Tarnow</t>
+          <t>Biala Podlaska</t>
         </is>
       </c>
       <c r="I91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J91" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>13/10/2023 02:13</t>
+        </is>
+      </c>
+      <c r="L91" t="n">
         <v>1.95</v>
       </c>
-      <c r="K91" t="inlineStr">
-        <is>
-          <t>14/10/2023 09:43</t>
-        </is>
-      </c>
-      <c r="L91" t="n">
-        <v>1.91</v>
-      </c>
       <c r="M91" t="inlineStr">
         <is>
-          <t>14/10/2023 14:47</t>
+          <t>14/10/2023 00:21</t>
         </is>
       </c>
       <c r="N91" t="n">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="O91" t="inlineStr">
         <is>
-          <t>14/10/2023 09:43</t>
+          <t>13/10/2023 02:13</t>
         </is>
       </c>
       <c r="P91" t="n">
-        <v>3.58</v>
+        <v>3.26</v>
       </c>
       <c r="Q91" t="inlineStr">
         <is>
-          <t>14/10/2023 14:47</t>
+          <t>14/10/2023 13:02</t>
         </is>
       </c>
       <c r="R91" t="n">
-        <v>3.18</v>
+        <v>2.83</v>
       </c>
       <c r="S91" t="inlineStr">
         <is>
-          <t>14/10/2023 09:43</t>
+          <t>13/10/2023 02:13</t>
         </is>
       </c>
       <c r="T91" t="n">
-        <v>3.31</v>
+        <v>3.44</v>
       </c>
       <c r="U91" t="inlineStr">
         <is>
-          <t>14/10/2023 14:47</t>
+          <t>14/10/2023 00:21</t>
         </is>
       </c>
       <c r="V91" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/swidniczanka-swidnik-unia-tarnow/hK2HFuun/</t>
+          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/star-starachowice-biala-podlaska/r9eUCwP4/</t>
         </is>
       </c>
     </row>
@@ -10785,22 +10785,22 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>Unia Tarnow</t>
+          <t>Orleta Radzyn</t>
         </is>
       </c>
       <c r="G113" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>Star Starachowice</t>
+          <t>Wislanie Jaskowice</t>
         </is>
       </c>
       <c r="I113" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J113" t="n">
-        <v>2.9</v>
+        <v>3.17</v>
       </c>
       <c r="K113" t="inlineStr">
         <is>
@@ -10808,15 +10808,15 @@
         </is>
       </c>
       <c r="L113" t="n">
-        <v>2.83</v>
+        <v>3.13</v>
       </c>
       <c r="M113" t="inlineStr">
         <is>
-          <t>04/11/2023 12:29</t>
+          <t>04/11/2023 12:40</t>
         </is>
       </c>
       <c r="N113" t="n">
-        <v>3.37</v>
+        <v>3.53</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -10824,15 +10824,15 @@
         </is>
       </c>
       <c r="P113" t="n">
-        <v>3.29</v>
+        <v>3.49</v>
       </c>
       <c r="Q113" t="inlineStr">
         <is>
-          <t>04/11/2023 12:29</t>
+          <t>04/11/2023 12:40</t>
         </is>
       </c>
       <c r="R113" t="n">
-        <v>1.98</v>
+        <v>1.82</v>
       </c>
       <c r="S113" t="inlineStr">
         <is>
@@ -10840,16 +10840,16 @@
         </is>
       </c>
       <c r="T113" t="n">
-        <v>2.23</v>
+        <v>2.01</v>
       </c>
       <c r="U113" t="inlineStr">
         <is>
-          <t>04/11/2023 12:29</t>
+          <t>04/11/2023 12:40</t>
         </is>
       </c>
       <c r="V113" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/unia-tarnow-star-starachowice/MiMHvmEE/</t>
+          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/orleta-radzyn-wislanie-jaskowice/foUVGqM7/</t>
         </is>
       </c>
     </row>
@@ -10877,22 +10877,22 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>Orleta Radzyn</t>
+          <t>Unia Tarnow</t>
         </is>
       </c>
       <c r="G114" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>Wislanie Jaskowice</t>
+          <t>Star Starachowice</t>
         </is>
       </c>
       <c r="I114" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J114" t="n">
-        <v>3.17</v>
+        <v>2.9</v>
       </c>
       <c r="K114" t="inlineStr">
         <is>
@@ -10900,15 +10900,15 @@
         </is>
       </c>
       <c r="L114" t="n">
-        <v>3.13</v>
+        <v>2.83</v>
       </c>
       <c r="M114" t="inlineStr">
         <is>
-          <t>04/11/2023 12:40</t>
+          <t>04/11/2023 12:29</t>
         </is>
       </c>
       <c r="N114" t="n">
-        <v>3.53</v>
+        <v>3.37</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
@@ -10916,15 +10916,15 @@
         </is>
       </c>
       <c r="P114" t="n">
-        <v>3.49</v>
+        <v>3.29</v>
       </c>
       <c r="Q114" t="inlineStr">
         <is>
-          <t>04/11/2023 12:40</t>
+          <t>04/11/2023 12:29</t>
         </is>
       </c>
       <c r="R114" t="n">
-        <v>1.82</v>
+        <v>1.98</v>
       </c>
       <c r="S114" t="inlineStr">
         <is>
@@ -10932,16 +10932,16 @@
         </is>
       </c>
       <c r="T114" t="n">
-        <v>2.01</v>
+        <v>2.23</v>
       </c>
       <c r="U114" t="inlineStr">
         <is>
-          <t>04/11/2023 12:40</t>
+          <t>04/11/2023 12:29</t>
         </is>
       </c>
       <c r="V114" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/orleta-radzyn-wislanie-jaskowice/foUVGqM7/</t>
+          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/unia-tarnow-star-starachowice/MiMHvmEE/</t>
         </is>
       </c>
     </row>
@@ -10969,22 +10969,22 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>Wisloka Debica</t>
+          <t>Podhale Nowy Targ</t>
         </is>
       </c>
       <c r="G115" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>Czarni Polaniec</t>
+          <t>Swidniczanka Swidnik</t>
         </is>
       </c>
       <c r="I115" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J115" t="n">
-        <v>2.04</v>
+        <v>1.93</v>
       </c>
       <c r="K115" t="inlineStr">
         <is>
@@ -10992,11 +10992,11 @@
         </is>
       </c>
       <c r="L115" t="n">
-        <v>2.02</v>
+        <v>2.09</v>
       </c>
       <c r="M115" t="inlineStr">
         <is>
-          <t>03/11/2023 15:19</t>
+          <t>04/11/2023 13:47</t>
         </is>
       </c>
       <c r="N115" t="n">
@@ -11008,15 +11008,15 @@
         </is>
       </c>
       <c r="P115" t="n">
-        <v>3.53</v>
+        <v>3.66</v>
       </c>
       <c r="Q115" t="inlineStr">
         <is>
-          <t>04/11/2023 12:00</t>
+          <t>04/11/2023 13:47</t>
         </is>
       </c>
       <c r="R115" t="n">
-        <v>2.74</v>
+        <v>2.97</v>
       </c>
       <c r="S115" t="inlineStr">
         <is>
@@ -11024,16 +11024,16 @@
         </is>
       </c>
       <c r="T115" t="n">
-        <v>3.01</v>
+        <v>2.84</v>
       </c>
       <c r="U115" t="inlineStr">
         <is>
-          <t>03/11/2023 15:19</t>
+          <t>04/11/2023 13:47</t>
         </is>
       </c>
       <c r="V115" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/wisloka-debica-czarni-polaniec/4GBMw7TK/</t>
+          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/podhale-nowy-targ-swidniczanka-swidnik/EkchYpir/</t>
         </is>
       </c>
     </row>
@@ -11061,22 +11061,22 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>Podhale Nowy Targ</t>
+          <t>Wisloka Debica</t>
         </is>
       </c>
       <c r="G116" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>Swidniczanka Swidnik</t>
+          <t>Czarni Polaniec</t>
         </is>
       </c>
       <c r="I116" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J116" t="n">
-        <v>1.93</v>
+        <v>2.04</v>
       </c>
       <c r="K116" t="inlineStr">
         <is>
@@ -11084,11 +11084,11 @@
         </is>
       </c>
       <c r="L116" t="n">
-        <v>2.09</v>
+        <v>2.02</v>
       </c>
       <c r="M116" t="inlineStr">
         <is>
-          <t>04/11/2023 13:47</t>
+          <t>03/11/2023 15:19</t>
         </is>
       </c>
       <c r="N116" t="n">
@@ -11100,15 +11100,15 @@
         </is>
       </c>
       <c r="P116" t="n">
-        <v>3.66</v>
+        <v>3.53</v>
       </c>
       <c r="Q116" t="inlineStr">
         <is>
-          <t>04/11/2023 13:47</t>
+          <t>04/11/2023 12:00</t>
         </is>
       </c>
       <c r="R116" t="n">
-        <v>2.97</v>
+        <v>2.74</v>
       </c>
       <c r="S116" t="inlineStr">
         <is>
@@ -11116,16 +11116,16 @@
         </is>
       </c>
       <c r="T116" t="n">
-        <v>2.84</v>
+        <v>3.01</v>
       </c>
       <c r="U116" t="inlineStr">
         <is>
-          <t>04/11/2023 13:47</t>
+          <t>03/11/2023 15:19</t>
         </is>
       </c>
       <c r="V116" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/podhale-nowy-targ-swidniczanka-swidnik/EkchYpir/</t>
+          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/wisloka-debica-czarni-polaniec/4GBMw7TK/</t>
         </is>
       </c>
     </row>
@@ -11429,7 +11429,7 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>Avia Swidnik</t>
+          <t>Star Starachowice</t>
         </is>
       </c>
       <c r="G120" t="n">
@@ -11437,63 +11437,63 @@
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>Wiazownica</t>
+          <t>Wisloka Debica</t>
         </is>
       </c>
       <c r="I120" t="n">
         <v>0</v>
       </c>
       <c r="J120" t="n">
-        <v>1.35</v>
+        <v>1.72</v>
       </c>
       <c r="K120" t="inlineStr">
         <is>
-          <t>11/11/2023 01:13</t>
+          <t>11/11/2023 02:12</t>
         </is>
       </c>
       <c r="L120" t="n">
-        <v>1.42</v>
+        <v>1.76</v>
       </c>
       <c r="M120" t="inlineStr">
         <is>
-          <t>11/11/2023 12:52</t>
+          <t>11/11/2023 12:22</t>
         </is>
       </c>
       <c r="N120" t="n">
-        <v>4.85</v>
+        <v>3.68</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
-          <t>11/11/2023 01:13</t>
+          <t>11/11/2023 02:12</t>
         </is>
       </c>
       <c r="P120" t="n">
-        <v>4.53</v>
+        <v>3.6</v>
       </c>
       <c r="Q120" t="inlineStr">
         <is>
-          <t>11/11/2023 12:52</t>
+          <t>11/11/2023 12:22</t>
         </is>
       </c>
       <c r="R120" t="n">
-        <v>5.72</v>
+        <v>3.71</v>
       </c>
       <c r="S120" t="inlineStr">
         <is>
-          <t>11/11/2023 01:13</t>
+          <t>11/11/2023 02:12</t>
         </is>
       </c>
       <c r="T120" t="n">
-        <v>5.46</v>
+        <v>3.81</v>
       </c>
       <c r="U120" t="inlineStr">
         <is>
-          <t>11/11/2023 12:52</t>
+          <t>11/11/2023 12:22</t>
         </is>
       </c>
       <c r="V120" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/avia-swidnik-wiazownica/hfyVo4Ls/</t>
+          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/star-starachowice-wisloka-debica/rVl9U2j7/</t>
         </is>
       </c>
     </row>
@@ -11521,71 +11521,71 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>Star Starachowice</t>
+          <t>Siarka Tarnobrzeg</t>
         </is>
       </c>
       <c r="G121" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>Wisloka Debica</t>
+          <t>Podhale Nowy Targ</t>
         </is>
       </c>
       <c r="I121" t="n">
         <v>0</v>
       </c>
       <c r="J121" t="n">
-        <v>1.72</v>
+        <v>1.45</v>
       </c>
       <c r="K121" t="inlineStr">
         <is>
-          <t>11/11/2023 02:12</t>
+          <t>11/11/2023 01:13</t>
         </is>
       </c>
       <c r="L121" t="n">
-        <v>1.76</v>
+        <v>1.49</v>
       </c>
       <c r="M121" t="inlineStr">
         <is>
-          <t>11/11/2023 12:22</t>
+          <t>11/11/2023 08:00</t>
         </is>
       </c>
       <c r="N121" t="n">
-        <v>3.68</v>
+        <v>4.33</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
-          <t>11/11/2023 02:12</t>
+          <t>11/11/2023 01:13</t>
         </is>
       </c>
       <c r="P121" t="n">
-        <v>3.6</v>
+        <v>4.15</v>
       </c>
       <c r="Q121" t="inlineStr">
         <is>
-          <t>11/11/2023 12:22</t>
+          <t>11/11/2023 11:03</t>
         </is>
       </c>
       <c r="R121" t="n">
-        <v>3.71</v>
+        <v>4.95</v>
       </c>
       <c r="S121" t="inlineStr">
         <is>
-          <t>11/11/2023 02:12</t>
+          <t>11/11/2023 01:13</t>
         </is>
       </c>
       <c r="T121" t="n">
-        <v>3.81</v>
+        <v>5.01</v>
       </c>
       <c r="U121" t="inlineStr">
         <is>
-          <t>11/11/2023 12:22</t>
+          <t>11/11/2023 08:00</t>
         </is>
       </c>
       <c r="V121" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/star-starachowice-wisloka-debica/rVl9U2j7/</t>
+          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/siarka-tarnobrzeg-podhale-nowy-targ/z5o1WOLf/</t>
         </is>
       </c>
     </row>
@@ -11613,22 +11613,22 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>Siarka Tarnobrzeg</t>
+          <t>Avia Swidnik</t>
         </is>
       </c>
       <c r="G122" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>Podhale Nowy Targ</t>
+          <t>Wiazownica</t>
         </is>
       </c>
       <c r="I122" t="n">
         <v>0</v>
       </c>
       <c r="J122" t="n">
-        <v>1.45</v>
+        <v>1.35</v>
       </c>
       <c r="K122" t="inlineStr">
         <is>
@@ -11636,15 +11636,15 @@
         </is>
       </c>
       <c r="L122" t="n">
-        <v>1.49</v>
+        <v>1.42</v>
       </c>
       <c r="M122" t="inlineStr">
         <is>
-          <t>11/11/2023 08:00</t>
+          <t>11/11/2023 12:52</t>
         </is>
       </c>
       <c r="N122" t="n">
-        <v>4.33</v>
+        <v>4.85</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -11652,15 +11652,15 @@
         </is>
       </c>
       <c r="P122" t="n">
-        <v>4.15</v>
+        <v>4.53</v>
       </c>
       <c r="Q122" t="inlineStr">
         <is>
-          <t>11/11/2023 11:03</t>
+          <t>11/11/2023 12:52</t>
         </is>
       </c>
       <c r="R122" t="n">
-        <v>4.95</v>
+        <v>5.72</v>
       </c>
       <c r="S122" t="inlineStr">
         <is>
@@ -11668,16 +11668,16 @@
         </is>
       </c>
       <c r="T122" t="n">
-        <v>5.01</v>
+        <v>5.46</v>
       </c>
       <c r="U122" t="inlineStr">
         <is>
-          <t>11/11/2023 08:00</t>
+          <t>11/11/2023 12:52</t>
         </is>
       </c>
       <c r="V122" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/siarka-tarnobrzeg-podhale-nowy-targ/z5o1WOLf/</t>
+          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/avia-swidnik-wiazownica/hfyVo4Ls/</t>
         </is>
       </c>
     </row>
@@ -12690,6 +12690,98 @@
       <c r="V133" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/ostrowiec-swietokrzyski-garbarnia/vobMGkDm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>poland</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>iii-liga-group-iv</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E134" s="2" t="n">
+        <v>45251.54166666666</v>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>Orleta Radzyn</t>
+        </is>
+      </c>
+      <c r="G134" t="n">
+        <v>1</v>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>Chelmianka Chelm</t>
+        </is>
+      </c>
+      <c r="I134" t="n">
+        <v>2</v>
+      </c>
+      <c r="J134" t="n">
+        <v>3.42</v>
+      </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>18/11/2023 01:13</t>
+        </is>
+      </c>
+      <c r="L134" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="M134" t="inlineStr">
+        <is>
+          <t>21/11/2023 12:59</t>
+        </is>
+      </c>
+      <c r="N134" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="O134" t="inlineStr">
+        <is>
+          <t>18/11/2023 01:13</t>
+        </is>
+      </c>
+      <c r="P134" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="Q134" t="inlineStr">
+        <is>
+          <t>21/11/2023 12:59</t>
+        </is>
+      </c>
+      <c r="R134" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="S134" t="inlineStr">
+        <is>
+          <t>18/11/2023 01:13</t>
+        </is>
+      </c>
+      <c r="T134" t="n">
+        <v>1.97</v>
+      </c>
+      <c r="U134" t="inlineStr">
+        <is>
+          <t>21/11/2023 12:59</t>
+        </is>
+      </c>
+      <c r="V134" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/poland/iii-liga-group-iv/orleta-radzyn-chelmianka-chelm/dM8HHVcs/</t>
         </is>
       </c>
     </row>

</xml_diff>